<commit_message>
[mnp] drawio - skills
</commit_message>
<xml_diff>
--- a/mnp/slg/MAP.SLG.Data.SkillData.xlsx
+++ b/mnp/slg/MAP.SLG.Data.SkillData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\map_docs\skills\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lazy_scripts\mnp\slg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="HeroSkill" sheetId="11" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="151">
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -476,6 +476,30 @@
   </si>
   <si>
     <t>Ref_Name</t>
+  </si>
+  <si>
+    <t>Heals HP by 50</t>
+  </si>
+  <si>
+    <t>Minor Heal</t>
+  </si>
+  <si>
+    <t>Heal 50 HP</t>
+  </si>
+  <si>
+    <t>Minor Regen</t>
+  </si>
+  <si>
+    <t>Heals HP by 50 for 4 turns</t>
+  </si>
+  <si>
+    <t>Heal 50 HP for 4 turns</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>Inflict 50 Damage for 4 turns</t>
   </si>
 </sst>
 </file>
@@ -771,7 +795,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -845,6 +869,7 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1408,8 +1433,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="tbl_heroskill" displayName="tbl_heroskill" ref="A1:N8" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" headerRowCellStyle="Note">
-  <autoFilter ref="A1:N8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="tbl_heroskill" displayName="tbl_heroskill" ref="A1:N11" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" headerRowCellStyle="Note">
+  <autoFilter ref="A1:N11"/>
   <tableColumns count="14">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -1876,8 +1901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15.75"/>
@@ -1965,35 +1990,35 @@
       </c>
       <c r="F2">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
         <v>141</v>
       </c>
       <c r="H2">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I2" t="s">
         <v>141</v>
       </c>
       <c r="J2">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_3]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K2" t="s">
         <v>141</v>
       </c>
       <c r="L2">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_4]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M2" t="s">
         <v>141</v>
       </c>
       <c r="N2">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_5]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -2015,35 +2040,35 @@
       </c>
       <c r="F3">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
         <v>140</v>
       </c>
       <c r="H3">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="J3">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_3]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="L3">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_4]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="N3">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_5]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -2065,35 +2090,35 @@
       </c>
       <c r="F4">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4" t="s">
         <v>141</v>
       </c>
       <c r="H4">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I4" t="s">
         <v>141</v>
       </c>
       <c r="J4">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_3]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K4" t="s">
         <v>141</v>
       </c>
       <c r="L4">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_4]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M4" t="s">
         <v>141</v>
       </c>
       <c r="N4">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_5]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -2115,35 +2140,35 @@
       </c>
       <c r="F5">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s">
         <v>140</v>
       </c>
       <c r="H5">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I5" t="s">
         <v>140</v>
       </c>
       <c r="J5">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_3]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K5" t="s">
         <v>140</v>
       </c>
       <c r="L5">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_4]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M5" t="s">
         <v>140</v>
       </c>
       <c r="N5">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_5]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -2165,35 +2190,35 @@
       </c>
       <c r="F6">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G6" t="s">
         <v>141</v>
       </c>
       <c r="H6">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I6" t="s">
         <v>141</v>
       </c>
       <c r="J6">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_3]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K6" t="s">
         <v>141</v>
       </c>
       <c r="L6">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_4]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M6" t="s">
         <v>141</v>
       </c>
       <c r="N6">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_5]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O6" s="5"/>
     </row>
@@ -2216,35 +2241,35 @@
       </c>
       <c r="F7">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G7" t="s">
         <v>140</v>
       </c>
       <c r="H7">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I7" t="s">
         <v>140</v>
       </c>
       <c r="J7">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_3]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K7" t="s">
         <v>140</v>
       </c>
       <c r="L7">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_4]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M7" t="s">
         <v>140</v>
       </c>
       <c r="N7">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_5]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -2266,33 +2291,180 @@
       </c>
       <c r="F8">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8" t="s">
         <v>141</v>
       </c>
       <c r="H8">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I8" t="s">
         <v>141</v>
       </c>
       <c r="J8">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_3]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K8" t="s">
         <v>141</v>
       </c>
       <c r="L8">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_4]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M8" t="s">
         <v>141</v>
       </c>
       <c r="N8">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_5]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9">
+        <v>100008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9" s="27">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>115</v>
+      </c>
+      <c r="J9">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_3]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>115</v>
+      </c>
+      <c r="L9" s="27">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_4]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>115</v>
+      </c>
+      <c r="N9">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_5]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10">
+        <v>100009</v>
+      </c>
+      <c r="B10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" s="27">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>115</v>
+      </c>
+      <c r="J10">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_3]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>115</v>
+      </c>
+      <c r="L10" s="27">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_4]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>115</v>
+      </c>
+      <c r="N10">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_5]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11">
+        <v>100010</v>
+      </c>
+      <c r="B11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="27">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_3]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>115</v>
+      </c>
+      <c r="L11" s="27">
+        <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_4]],SubSkill!$B$2:$B$1000,0))</f>
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>115</v>
+      </c>
+      <c r="N11">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_heroskill[[#This Row],[Ref_SubSkill_5]],SubSkill!$B$2:$B$1000,0))</f>
         <v>0</v>
       </c>
@@ -2313,7 +2485,7 @@
           <x14:formula1>
             <xm:f>SubSkill!$B$2:$B$1000</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K8 E2:E8 G2:G8 I2:I8 M2:M8</xm:sqref>
+          <xm:sqref>E2:E11 G2:G11 M2:M11 I2:I11 K2:K11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2417,7 +2589,7 @@
       </c>
       <c r="F2">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_weaponskill[[#This Row],[Ref_SubSkill_1]],SubSkill!$B$2:$B$1000,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H2" t="e">
         <f>INDEX(SubSkill!$A$2:$A$1000,MATCH(tbl_weaponskill[[#This Row],[Ref_SubSkill_2]],SubSkill!$B$2:$B$1000,0))</f>
@@ -2703,8 +2875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15.75"/>
@@ -2792,31 +2964,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D2">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_TargetType]],tbl_targettype[[target_type]:[id]],2,FALSE),"-1")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="F2">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P1_ValueType]],tbl_valuetype[[value_type]:[id]],2,FALSE),"-1")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="H2">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P1_FieldType]],tbl_fieldtype[[field_type]:[id]],2,FALSE),"-1")</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="J2" t="s">
         <v>116</v>
@@ -2858,31 +3030,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_TargetType]],tbl_targettype[[target_type]:[id]],2,FALSE),"-1")</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P1_ValueType]],tbl_valuetype[[value_type]:[id]],2,FALSE),"-1")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H3">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P1_FieldType]],tbl_fieldtype[[field_type]:[id]],2,FALSE),"-1")</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>170</v>
+        <v>50</v>
       </c>
       <c r="J3" t="s">
         <v>116</v>
@@ -2924,48 +3096,48 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_TargetType]],tbl_targettype[[target_type]:[id]],2,FALSE),"-1")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P1_ValueType]],tbl_valuetype[[value_type]:[id]],2,FALSE),"-1")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H4">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P1_FieldType]],tbl_fieldtype[[field_type]:[id]],2,FALSE),"-1")</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I4">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="J4" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="K4">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P2_ValueType]],tbl_valuetype[[value_type]:[id]],2,FALSE),"-1")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="M4">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P2_FieldType]],tbl_fieldtype[[field_type]:[id]],2,FALSE),"-1")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O4" t="s">
         <v>116</v>
@@ -2990,21 +3162,21 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_TargetType]],tbl_targettype[[target_type]:[id]],2,FALSE),"-1")</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P1_ValueType]],tbl_valuetype[[value_type]:[id]],2,FALSE),"-1")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
         <v>92</v>
@@ -3014,24 +3186,24 @@
         <v>9</v>
       </c>
       <c r="I5">
-        <v>170</v>
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="K5">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P2_ValueType]],tbl_valuetype[[value_type]:[id]],2,FALSE),"-1")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="M5">
         <f>IFERROR(VLOOKUP(tbl_subskill[[#This Row],[Ref_P2_FieldType]],tbl_fieldtype[[field_type]:[id]],2,FALSE),"-1")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O5" t="s">
         <v>116</v>

</xml_diff>